<commit_message>
Changed J to mJ in figures
</commit_message>
<xml_diff>
--- a/Documents/ExperimentMetrics.xlsx
+++ b/Documents/ExperimentMetrics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\workspace\DEVS_Suite_3.0.0_mixed_win64\DEVS_Suite_3.0.0_mixed_win64\src\cse561\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\DEVSWorkspace\DEVS\src\cse561\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="23">
   <si>
     <t>Level</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Payload bytes</t>
   </si>
   <si>
-    <t>Level 3 - Hash (J)</t>
-  </si>
-  <si>
     <t>1024 B</t>
   </si>
   <si>
@@ -81,19 +78,25 @@
     <t>0 B</t>
   </si>
   <si>
-    <t>Level 1 (J)</t>
-  </si>
-  <si>
-    <t>Level 2 (J)</t>
-  </si>
-  <si>
-    <t>Level 3 (J)</t>
-  </si>
-  <si>
     <t>Bytes</t>
   </si>
   <si>
-    <t>Level 3 -Assymetric Encryption (J)</t>
+    <t>Level 1 (mJ)</t>
+  </si>
+  <si>
+    <t>Power (mJ)</t>
+  </si>
+  <si>
+    <t>Level 2 (mJ)</t>
+  </si>
+  <si>
+    <t>Level 3 (mJ)</t>
+  </si>
+  <si>
+    <t>Level 3 - Hash (mJ)</t>
+  </si>
+  <si>
+    <t>Level 3 -Assymetric Encryption (mJ)</t>
   </si>
 </sst>
 </file>
@@ -277,7 +280,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Joule Usage</a:t>
+              <a:t> milli-Joule Usage</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -336,7 +339,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="1">
-                  <c:v>Level 1 (J)</c:v>
+                  <c:v>Level 1 (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -468,7 +471,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="1">
-                  <c:v>Level 2 (J)</c:v>
+                  <c:v>Level 2 (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -600,11 +603,11 @@
         </c:dLbls>
         <c:gapWidth val="98"/>
         <c:overlap val="-15"/>
-        <c:axId val="324836608"/>
-        <c:axId val="324834256"/>
+        <c:axId val="440746240"/>
+        <c:axId val="440746632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324836608"/>
+        <c:axId val="440746240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324834256"/>
+        <c:crossAx val="440746632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -655,7 +658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324834256"/>
+        <c:axId val="440746632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000"/>
@@ -707,7 +710,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324836608"/>
+        <c:crossAx val="440746240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -823,7 +826,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Total Power</a:t>
+              <a:t>Total Energy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -881,7 +884,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Level 1 (J)</c:v>
+                  <c:v>Level 1 (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1012,7 +1015,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Level 2 (J)</c:v>
+                  <c:v>Level 2 (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1143,7 +1146,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Level 3 (J)</c:v>
+                  <c:v>Level 3 (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1275,11 +1278,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="324832688"/>
-        <c:axId val="324835824"/>
+        <c:axId val="440748200"/>
+        <c:axId val="440752512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324832688"/>
+        <c:axId val="440748200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324835824"/>
+        <c:crossAx val="440752512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1330,7 +1333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324835824"/>
+        <c:axId val="440752512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000"/>
@@ -1382,7 +1385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324832688"/>
+        <c:crossAx val="440748200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1531,7 +1534,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Level 3 - Hash (J)</c:v>
+                  <c:v>Level 3 - Hash (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1662,11 +1665,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="324827984"/>
-        <c:axId val="324827592"/>
+        <c:axId val="440751336"/>
+        <c:axId val="440758392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324827984"/>
+        <c:axId val="440751336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +1712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324827592"/>
+        <c:crossAx val="440758392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1717,7 +1720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324827592"/>
+        <c:axId val="440758392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4000"/>
@@ -1769,7 +1772,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324827984"/>
+        <c:crossAx val="440751336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1886,7 +1889,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Level 3 -Assymetric Encryption (J)</c:v>
+                  <c:v>Level 3 -Assymetric Encryption (mJ)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2017,11 +2020,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="324837392"/>
-        <c:axId val="324828376"/>
+        <c:axId val="440759960"/>
+        <c:axId val="440760352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324837392"/>
+        <c:axId val="440759960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,7 +2067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324828376"/>
+        <c:crossAx val="440760352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2072,7 +2075,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324828376"/>
+        <c:axId val="440760352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15500"/>
@@ -2124,7 +2127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324837392"/>
+        <c:crossAx val="440759960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4735,7 +4738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -5099,12 +5102,12 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -5194,16 +5197,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>
@@ -5211,13 +5214,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -5350,7 +5353,7 @@
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -5489,7 +5492,7 @@
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -5634,7 +5637,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -5642,12 +5645,12 @@
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1">
         <v>6650.1</v>
@@ -5658,7 +5661,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="1">
         <v>8308.98</v>
@@ -5669,7 +5672,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1">
         <v>9967.86</v>
@@ -5680,7 +5683,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1">
         <v>11626.74</v>
@@ -5691,7 +5694,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="1">
         <v>13285.62</v>
@@ -5704,7 +5707,7 @@
       <c r="B29" s="7"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>10</v>
       </c>
@@ -5712,15 +5715,15 @@
         <v>17</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="4">
         <v>6650.1</v>
@@ -5734,7 +5737,7 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="4">
         <v>8308.98</v>
@@ -5748,7 +5751,7 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="4">
         <v>9967.86</v>
@@ -5762,7 +5765,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35" s="4">
         <v>11626.74</v>
@@ -5776,7 +5779,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" s="4">
         <v>13285.62</v>
@@ -5794,12 +5797,12 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B40" s="2">
         <v>6041.6</v>
@@ -5807,7 +5810,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B41" s="2">
         <v>12083.2</v>
@@ -5815,7 +5818,7 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" s="2">
         <v>18124.8</v>
@@ -5823,7 +5826,7 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" s="2">
         <v>24166.400000000001</v>
@@ -5831,7 +5834,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B44" s="2">
         <v>30208</v>
@@ -5843,12 +5846,12 @@
         <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B47" s="2">
         <v>15564.8</v>
@@ -5856,7 +5859,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B48" s="2">
         <v>16185.98</v>
@@ -5864,7 +5867,7 @@
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" s="2">
         <v>16795.259999999998</v>
@@ -5872,7 +5875,7 @@
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B50" s="2">
         <v>17404.54</v>
@@ -5880,7 +5883,7 @@
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B51" s="2">
         <v>18013.82</v>

</xml_diff>

<commit_message>
Small tweak to data label on graph
</commit_message>
<xml_diff>
--- a/Documents/ExperimentMetrics.xlsx
+++ b/Documents/ExperimentMetrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\workspace\DEVS_Suite_3.0.0_mixed_win64\DEVS_Suite_3.0.0_mixed_win64\src\cse561\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -367,7 +367,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0;\-#,##0" sourceLinked="0"/>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -615,11 +615,11 @@
         </c:dLbls>
         <c:gapWidth val="98"/>
         <c:overlap val="-15"/>
-        <c:axId val="324350384"/>
-        <c:axId val="324351560"/>
+        <c:axId val="324962400"/>
+        <c:axId val="324964752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324350384"/>
+        <c:axId val="324962400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,7 +662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324351560"/>
+        <c:crossAx val="324964752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -670,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324351560"/>
+        <c:axId val="324964752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000"/>
@@ -722,7 +722,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324350384"/>
+        <c:crossAx val="324962400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1290,11 +1290,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="324352344"/>
-        <c:axId val="324352736"/>
+        <c:axId val="324965928"/>
+        <c:axId val="324959656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324352344"/>
+        <c:axId val="324965928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324352736"/>
+        <c:crossAx val="324959656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,7 +1345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324352736"/>
+        <c:axId val="324959656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000"/>
@@ -1397,7 +1397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324352344"/>
+        <c:crossAx val="324965928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1677,11 +1677,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="324353128"/>
-        <c:axId val="324347248"/>
+        <c:axId val="326403960"/>
+        <c:axId val="326403176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324353128"/>
+        <c:axId val="326403960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1724,7 +1724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324347248"/>
+        <c:crossAx val="326403176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1732,7 +1732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324347248"/>
+        <c:axId val="326403176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1784,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324353128"/>
+        <c:crossAx val="326403960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2032,11 +2032,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="326108400"/>
-        <c:axId val="326105656"/>
+        <c:axId val="326409056"/>
+        <c:axId val="326410232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="326108400"/>
+        <c:axId val="326409056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326105656"/>
+        <c:crossAx val="326410232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2087,7 +2087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="326105656"/>
+        <c:axId val="326410232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15500"/>
@@ -2139,7 +2139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326108400"/>
+        <c:crossAx val="326409056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5209,8 +5209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated results and bug fixes
</commit_message>
<xml_diff>
--- a/Documents/ExperimentMetrics.xlsx
+++ b/Documents/ExperimentMetrics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\workspace\DEVS_Suite_3.0.0_mixed_win64\DEVS_Suite_3.0.0_mixed_win64\src\cse561\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\DEVSWorkspace\DEVS\src\cse561\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -615,11 +615,11 @@
         </c:dLbls>
         <c:gapWidth val="98"/>
         <c:overlap val="-15"/>
-        <c:axId val="324962400"/>
-        <c:axId val="324964752"/>
+        <c:axId val="436607120"/>
+        <c:axId val="436612216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324962400"/>
+        <c:axId val="436607120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,7 +662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324964752"/>
+        <c:crossAx val="436612216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -670,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324964752"/>
+        <c:axId val="436612216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000"/>
@@ -722,7 +722,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324962400"/>
+        <c:crossAx val="436607120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1262,19 +1262,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15570.8416</c:v>
+                  <c:v>615.32159999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16198.063200000001</c:v>
+                  <c:v>16490.163199999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16813.3848</c:v>
+                  <c:v>32061.004799999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17428.706399999999</c:v>
+                  <c:v>47631.845999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18044.28</c:v>
+                  <c:v>63202.688000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,11 +1290,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="324965928"/>
-        <c:axId val="324959656"/>
+        <c:axId val="436610256"/>
+        <c:axId val="436610648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="324965928"/>
+        <c:axId val="436610256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324959656"/>
+        <c:crossAx val="436610648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,7 +1345,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324959656"/>
+        <c:axId val="436610648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6000"/>
@@ -1397,7 +1397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324965928"/>
+        <c:crossAx val="436610256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1677,11 +1677,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="326403960"/>
-        <c:axId val="326403176"/>
+        <c:axId val="436612608"/>
+        <c:axId val="436611040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="326403960"/>
+        <c:axId val="436612608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1724,7 +1724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326403176"/>
+        <c:crossAx val="436611040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1732,7 +1732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="326403176"/>
+        <c:axId val="436611040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1784,7 +1784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326403960"/>
+        <c:crossAx val="436612608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2004,19 +2004,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15564.8</c:v>
+                  <c:v>609.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16185.98</c:v>
+                  <c:v>16478.080000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16795.259999999998</c:v>
+                  <c:v>32042.879000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17404.54</c:v>
+                  <c:v>47607.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18013.82</c:v>
+                  <c:v>63172.480000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,11 +2032,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="326409056"/>
-        <c:axId val="326410232"/>
+        <c:axId val="441568680"/>
+        <c:axId val="441561232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="326409056"/>
+        <c:axId val="441568680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326410232"/>
+        <c:crossAx val="441561232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2087,7 +2087,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="326410232"/>
+        <c:axId val="441561232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="15500"/>
@@ -2139,7 +2139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326409056"/>
+        <c:crossAx val="441568680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5209,8 +5209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5533,10 +5533,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="2">
-        <v>15570.8416</v>
+        <v>615.32159999999999</v>
       </c>
       <c r="D16" s="2">
-        <v>15564.8</v>
+        <v>609.28</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -5556,10 +5556,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="2">
-        <v>16198.063200000001</v>
+        <v>16490.163199999999</v>
       </c>
       <c r="D17" s="2">
-        <v>16185.98</v>
+        <v>16478.080000000002</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -5579,10 +5579,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>16813.3848</v>
+        <v>32061.004799999999</v>
       </c>
       <c r="D18" s="2">
-        <v>16795.259999999998</v>
+        <v>32042.879000000001</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -5602,10 +5602,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="2">
-        <v>17428.706399999999</v>
+        <v>47631.845999999998</v>
       </c>
       <c r="D19" s="2">
-        <v>17404.54</v>
+        <v>47607.68</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -5625,10 +5625,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="2">
-        <v>18044.28</v>
+        <v>63202.688000000002</v>
       </c>
       <c r="D20" s="2">
-        <v>18013.82</v>
+        <v>63172.480000000003</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -5649,7 +5649,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -5744,7 +5744,8 @@
         <v>6655.1</v>
       </c>
       <c r="D32" s="2">
-        <v>15570.8416</v>
+        <f>C16</f>
+        <v>615.32159999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5758,7 +5759,8 @@
         <v>8313.98</v>
       </c>
       <c r="D33" s="2">
-        <v>16198.063200000001</v>
+        <f>C17</f>
+        <v>16490.163199999999</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5772,7 +5774,8 @@
         <v>9972.86</v>
       </c>
       <c r="D34" s="2">
-        <v>16813.3848</v>
+        <f>C18</f>
+        <v>32061.004799999999</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5786,7 +5789,8 @@
         <v>11631.74</v>
       </c>
       <c r="D35" s="2">
-        <v>17428.706399999999</v>
+        <f>C19</f>
+        <v>47631.845999999998</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5800,7 +5804,8 @@
         <v>13290.62</v>
       </c>
       <c r="D36" s="2">
-        <v>18044.28</v>
+        <f>C20</f>
+        <v>63202.688000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5866,7 +5871,8 @@
         <v>15</v>
       </c>
       <c r="B47" s="2">
-        <v>15564.8</v>
+        <f>D16</f>
+        <v>609.28</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5874,7 +5880,8 @@
         <v>11</v>
       </c>
       <c r="B48" s="2">
-        <v>16185.98</v>
+        <f>D17</f>
+        <v>16478.080000000002</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5882,7 +5889,8 @@
         <v>12</v>
       </c>
       <c r="B49" s="2">
-        <v>16795.259999999998</v>
+        <f>D18</f>
+        <v>32042.879000000001</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5890,7 +5898,8 @@
         <v>13</v>
       </c>
       <c r="B50" s="2">
-        <v>17404.54</v>
+        <f>D19</f>
+        <v>47607.68</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5898,7 +5907,8 @@
         <v>14</v>
       </c>
       <c r="B51" s="2">
-        <v>18013.82</v>
+        <f>D20</f>
+        <v>63172.480000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>